<commit_message>
Updated dbCAN EC matches
</commit_message>
<xml_diff>
--- a/dbcan/sig_cazymes_info.xlsx
+++ b/dbcan/sig_cazymes_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{3EB5E469-630B-420F-995B-064CD9BDD0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D2B4BAC-E09E-4C5C-84AA-FF01792957A0}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{3EB5E469-630B-420F-995B-064CD9BDD0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BF68FA8-6A9C-4C8F-B5B5-50100F7750C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1D7D89D5-1344-43D6-9395-CBB1D300203F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D7D89D5-1344-43D6-9395-CBB1D300203F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
   <si>
     <t>GT101</t>
   </si>
@@ -138,9 +138,6 @@
     <t>β-glucosyltransferase </t>
   </si>
   <si>
-    <t>CAZy</t>
-  </si>
-  <si>
     <t>Family built after PMID=25023666; The GT101 module of Streptococcus parasanguinis dGT1 catalyzes the transfer of b-glucose to the branch point of the hexasaccharide O-linked to the serine-rich repeat of the bacterial adhesin Fap1.</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>UDP-GlcNAc: peptide β-N-acetylglucosaminyltransferase (EC 2.4.1.255); UDP-Glc: peptide N-β-glucosyltransferase (EC 2.4.1.-)</t>
   </si>
   <si>
-    <t>Final</t>
-  </si>
-  <si>
     <t>pectin / pectate lyase</t>
   </si>
   <si>
@@ -219,27 +213,15 @@
     <t>Involved in biofilm formation (modifies bacterial adhesin Fap1)</t>
   </si>
   <si>
-    <t>Glycogen synthase - does this help microbes survive hib because glycogen is an NRG source for microbes?</t>
-  </si>
-  <si>
-    <t>Mucin deg</t>
-  </si>
-  <si>
     <t>Involved in LPS synthesis (Lipid A)</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Galactocerebrosidase is in humans</t>
-  </si>
-  <si>
     <t>B-galactosidase</t>
   </si>
   <si>
-    <t>Xylan deg</t>
-  </si>
-  <si>
     <t>Xylan / xylose deg</t>
   </si>
   <si>
@@ -256,6 +238,147 @@
   </si>
   <si>
     <t>Iduronidase is in humans</t>
+  </si>
+  <si>
+    <t>3.5.1.108</t>
+  </si>
+  <si>
+    <t>3.2.1.21</t>
+  </si>
+  <si>
+    <t>3.2.1.37</t>
+  </si>
+  <si>
+    <t>3.2.1.52</t>
+  </si>
+  <si>
+    <t>3.2.1.55</t>
+  </si>
+  <si>
+    <t>3.2.1.4</t>
+  </si>
+  <si>
+    <t>3.2.1.8</t>
+  </si>
+  <si>
+    <t>3.2.1.23</t>
+  </si>
+  <si>
+    <t>3.2.1.4 not in winter</t>
+  </si>
+  <si>
+    <t>3.2.1.8 in all</t>
+  </si>
+  <si>
+    <t>2.4.1.11</t>
+  </si>
+  <si>
+    <t>3.2.1.26</t>
+  </si>
+  <si>
+    <t>3.2.1.65</t>
+  </si>
+  <si>
+    <t>3.2.1.80</t>
+  </si>
+  <si>
+    <t>3.2.1.153</t>
+  </si>
+  <si>
+    <t>2.4.1.99</t>
+  </si>
+  <si>
+    <t>2.4.1.100</t>
+  </si>
+  <si>
+    <t>2.4.1.243</t>
+  </si>
+  <si>
+    <t>3.2.1.7</t>
+  </si>
+  <si>
+    <t>3.2.1.35</t>
+  </si>
+  <si>
+    <t>3.2.1.169</t>
+  </si>
+  <si>
+    <t>Seasons</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Is 3.2.1.46 only mammalian?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endo-β-1,4-glucanase </t>
+  </si>
+  <si>
+    <t>endo-1,4-β-xylanase</t>
+  </si>
+  <si>
+    <t>β-glucosidase</t>
+  </si>
+  <si>
+    <t>xylan 1,4-β-xylosidase</t>
+  </si>
+  <si>
+    <t>β-N-acetylhexosaminidase</t>
+  </si>
+  <si>
+    <t>α-L-arabinofuranosidase</t>
+  </si>
+  <si>
+    <t>invertase</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>endo-levanase</t>
+  </si>
+  <si>
+    <t>endo-inulinase</t>
+  </si>
+  <si>
+    <t>fructan:fructan 6G-fructosyltransferase</t>
+  </si>
+  <si>
+    <t>fructan:fructan 1-fructosyltransferase</t>
+  </si>
+  <si>
+    <t>exo-inulinase</t>
+  </si>
+  <si>
+    <t>ructan β-(2,1)-fructosidase/1-exohydrolase</t>
+  </si>
+  <si>
+    <t>β-xylosidase</t>
+  </si>
+  <si>
+    <t>β-galactosidase</t>
+  </si>
+  <si>
+    <t>β-hexosaminidase</t>
+  </si>
+  <si>
+    <t>hyaluronidase</t>
+  </si>
+  <si>
+    <t>[protein]-3-O-(GlcNAc)-L-Ser/Thr β-N-acetylglucosaminidase</t>
+  </si>
+  <si>
+    <t>Glycogen synthase</t>
+  </si>
+  <si>
+    <t>Does this help microbes survive hib because glycogen is an NRG source for microbes?</t>
+  </si>
+  <si>
+    <t>UDP-3-0-acyl N-acetylglucosamine deacetylase</t>
+  </si>
+  <si>
+    <t>CAZy Entry</t>
   </si>
 </sst>
 </file>
@@ -279,18 +402,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -305,12 +422,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,15 +741,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E237DDC-612D-435C-B42D-9015223A018E}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A2:G8"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="6.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -644,19 +766,25 @@
         <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -670,14 +798,19 @@
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -688,17 +821,20 @@
         <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -709,53 +845,62 @@
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
@@ -764,17 +909,20 @@
         <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -783,243 +931,528 @@
         <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s">
-        <v>73</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated docs w/ eCAMI info
</commit_message>
<xml_diff>
--- a/dbcan/sig_cazymes_info.xlsx
+++ b/dbcan/sig_cazymes_info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/OG_MetaG/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{3EB5E469-630B-420F-995B-064CD9BDD0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BF68FA8-6A9C-4C8F-B5B5-50100F7750C6}"/>
+  <xr:revisionPtr revIDLastSave="1149" documentId="8_{3EB5E469-630B-420F-995B-064CD9BDD0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B4B49D3A-7CE8-4C94-BDA8-792D9B6DB409}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D7D89D5-1344-43D6-9395-CBB1D300203F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1D7D89D5-1344-43D6-9395-CBB1D300203F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="324">
   <si>
     <t>GT101</t>
   </si>
@@ -379,13 +380,640 @@
   </si>
   <si>
     <t>CAZy Entry</t>
+  </si>
+  <si>
+    <t>Family built after PMID=25023666; The GT101 module of Streptococcus parasanguinis dGT1 catalyzes the transfer of b-glucose to the branch point of the hexasaccharide O-linked to the serine-rich repeat of the bacterial adhesin Fap1. Fap1 confers rapamycin resistance</t>
+  </si>
+  <si>
+    <t>Involved in biofilm formation (modifies bacterial adhesin Fap1). Confers rapamycin resistance</t>
+  </si>
+  <si>
+    <t>Citation</t>
+  </si>
+  <si>
+    <t>Wu 1998; Froeliger 2001; Wu 2007</t>
+  </si>
+  <si>
+    <t>Summer &gt; Spring; Summer &gt; Winter</t>
+  </si>
+  <si>
+    <t>galactocerebrosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.23</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.46</t>
+  </si>
+  <si>
+    <t>Summer &gt; Winter</t>
+  </si>
+  <si>
+    <t>EC 4.2.2.2</t>
+  </si>
+  <si>
+    <t>pectate lyase</t>
+  </si>
+  <si>
+    <t>exo-pectate lyase</t>
+  </si>
+  <si>
+    <t>EC 4.2.2.9</t>
+  </si>
+  <si>
+    <t>pectin lyase</t>
+  </si>
+  <si>
+    <t>EC 4.2.2.10</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Pectate degradation</t>
+  </si>
+  <si>
+    <t>Summer &gt; Winter; Spring &gt; Winter</t>
+  </si>
+  <si>
+    <t>In all samples</t>
+  </si>
+  <si>
+    <t>Not in winter; in 2 summer and 2 spring</t>
+  </si>
+  <si>
+    <t>Degrades xylan</t>
+  </si>
+  <si>
+    <t>Degrades cellulose, lichenin and cereal β-D-glucans</t>
+  </si>
+  <si>
+    <t>In all samples. Xylan is 2nd most abundant structural polysaccharide in plant cell walls; it's particularly high in cereal grains</t>
+  </si>
+  <si>
+    <t>Zhang 2014</t>
+  </si>
+  <si>
+    <t>xylan α-1,2-glucuronidase</t>
+  </si>
+  <si>
+    <t>α-(4-O-methyl)-glucuronidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.131</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.-</t>
+  </si>
+  <si>
+    <t>Degrades major chain of hardwood xylans</t>
+  </si>
+  <si>
+    <t>Rogowski 2014</t>
+  </si>
+  <si>
+    <t>pectin acetylesterase</t>
+  </si>
+  <si>
+    <t>EC 3.1.1.-</t>
+  </si>
+  <si>
+    <t>rhamnogalacturonan acetylesterase</t>
+  </si>
+  <si>
+    <t>acetyl xylan esterase</t>
+  </si>
+  <si>
+    <t>EC 3.1.1.72</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.37</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.55</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.8</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.-</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.99</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.146</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.145</t>
+  </si>
+  <si>
+    <t>α-1,2-L-arabinofuranosidase</t>
+  </si>
+  <si>
+    <t>exo-α-1,5-L-arabinofuranosidase</t>
+  </si>
+  <si>
+    <t>[inverting] exo-α-1,5-L-arabinanase</t>
+  </si>
+  <si>
+    <t>β-1,3-xylosidase</t>
+  </si>
+  <si>
+    <t>[inverting] endo-α-1,5-L-arabinanase</t>
+  </si>
+  <si>
+    <t>exo-β-1,3-galactanase</t>
+  </si>
+  <si>
+    <t>β-D-galactofuranosidase</t>
+  </si>
+  <si>
+    <t>Degrades xylose and xylobiose</t>
+  </si>
+  <si>
+    <t>Degrades α-L-arabinofuranosides, α-L-arabinans containing (1,3)- and/or (1,5)-linkages, arabinoxylans and arabinogalactans</t>
+  </si>
+  <si>
+    <t>xylanase</t>
+  </si>
+  <si>
+    <t>Acts best on linear 1,5-α-L-arabinan. Also acts on branched arabinan, but more slowly.</t>
+  </si>
+  <si>
+    <t>Removes not only free galactose, but also 6-glycosylated residues; releases branches from [arabino-galacto-(1→6)]-(1→3)-β-D-galactans.</t>
+  </si>
+  <si>
+    <t>Steiner 1971</t>
+  </si>
+  <si>
+    <t>Fungal plant path enzyme (Helminthosporium sacchari, infects sugar cane); detoxifies helminthosporoside (a host-specific toxin produced by fungus)</t>
+  </si>
+  <si>
+    <t>Spring &gt; Winter</t>
+  </si>
+  <si>
+    <t>GH3 not in 3715 (summer). 3.2.1.21 found in all squirrels w/ GH3</t>
+  </si>
+  <si>
+    <t>Found in all squirrels w/ GH3</t>
+  </si>
+  <si>
+    <t>Not found in 1 winter, 2 spring</t>
+  </si>
+  <si>
+    <t>Wide specificity for β-D-glucosides</t>
+  </si>
+  <si>
+    <t>Acts on N-acetylglucosides and N-acetylgalactosides.</t>
+  </si>
+  <si>
+    <t>Acts on α-L-arabinofuranosides, α-L-arabinans containing (1,3)- and/or (1,5)-linkages, arabinoxylans and arabinogalactans</t>
+  </si>
+  <si>
+    <t>endo-β-1,4-glucanase / cellulase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.4</t>
+  </si>
+  <si>
+    <t>endo-β-1,4-xylanase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.21</t>
+  </si>
+  <si>
+    <t>β-mannosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.25</t>
+  </si>
+  <si>
+    <t>β-glucosylceramidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.45</t>
+  </si>
+  <si>
+    <t>glucan β-1,3-glucosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.58</t>
+  </si>
+  <si>
+    <t>exo-β-1,4-glucanase / cellodextrinase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.74</t>
+  </si>
+  <si>
+    <t>glucan endo-1,6-β-glucosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.75</t>
+  </si>
+  <si>
+    <t>mannan endo-β-1,4-mannosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.78</t>
+  </si>
+  <si>
+    <t>cellulose β-1,4-cellobiosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.91</t>
+  </si>
+  <si>
+    <t>steryl β-glucosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.104</t>
+  </si>
+  <si>
+    <t>endoglycoceramidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.123</t>
+  </si>
+  <si>
+    <t>chitosanase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.132</t>
+  </si>
+  <si>
+    <t>β-primeverosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.149</t>
+  </si>
+  <si>
+    <t>xyloglucan-specific endo-β-1,4-glucanase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.151</t>
+  </si>
+  <si>
+    <t>endo-β-1,6-galactanase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.164</t>
+  </si>
+  <si>
+    <t>β-1,3-mannanase</t>
+  </si>
+  <si>
+    <t>arabinoxylan-specific endo-β-1,4-xylanase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.-</t>
+  </si>
+  <si>
+    <t>mannan transglycosylase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.73</t>
+  </si>
+  <si>
+    <t>lichenase / endo-β-1,3-1,4-glucanase</t>
+  </si>
+  <si>
+    <t>β-glycosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.39</t>
+  </si>
+  <si>
+    <t>endo-β-1,3-glucanase / laminarinase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.52</t>
+  </si>
+  <si>
+    <t>β-galactosylceramidase</t>
+  </si>
+  <si>
+    <t>β-rutinosidase /α-L-rhamnose-(1,6)-β-D-glucosidase</t>
+  </si>
+  <si>
+    <t>glucomannan-specific endo-Î²-1,4-glucanase</t>
+  </si>
+  <si>
+    <t>Degrades xylans</t>
+  </si>
+  <si>
+    <t>Degrades glucosylceramide and glucosylsphingosine</t>
+  </si>
+  <si>
+    <t>Acts on oligosaccharides, but very slowly on laminaribiose</t>
+  </si>
+  <si>
+    <t>Acts on 1,4-β-D-glucans and related oligosaccharides. Cellobiose is hydrolysed, but very slowly</t>
+  </si>
+  <si>
+    <t>Acts on lutean, pustulan and 1,6-oligo-β-D-glucosides</t>
+  </si>
+  <si>
+    <t>Degrades mannans, galactomannans and glucomannans</t>
+  </si>
+  <si>
+    <t>Acts on glucosides of cholesterol and sitosterol, but not on some related sterols such as coprostanol</t>
+  </si>
+  <si>
+    <t>Degrades acidic and neutral glycosphingolipids to oligosaccharides and ceramides. Doesn't act on monoglycosylceramides</t>
+  </si>
+  <si>
+    <t>Specific for xyloglucan. Doesn't hydrolyse other cell-wall components</t>
+  </si>
+  <si>
+    <t>Forms of the alcoholic aroma in oolong and black tea</t>
+  </si>
+  <si>
+    <t>Specifically hydrolyses 1,6-β-D-galactooligosaccharides with a degree of polymerization (DP) higher than 3, and their acidic derivatives with 4-O-methylglucosyluronate or glucosyluronate groups at the non-reducing terminals. Can also hydrolyse α-L-arabinofuranosidase-treated arabinogalactan protein (AGP). AGPs are involved in many physiological events (e.g. cell division, cell expansion and cell death)</t>
+  </si>
+  <si>
+    <t>Degrades lichenin and cereal β-D-glucans, but not β-D-glucans containing only 1,3- or 1,4-bonds</t>
+  </si>
+  <si>
+    <t>Degrades α-L-arabinofuranosides, α-L-arabinans containing (1,3)- and/or (1,5)-linkages, arabinoxylans and arabinogalactans</t>
+  </si>
+  <si>
+    <t>Not in 2 winter, 1 spring</t>
+  </si>
+  <si>
+    <t>Not in 1 winter</t>
+  </si>
+  <si>
+    <t>In 1 summer, 1 winter</t>
+  </si>
+  <si>
+    <t>In 1 winter, 1 spring</t>
+  </si>
+  <si>
+    <t>In 3 spring</t>
+  </si>
+  <si>
+    <t>sucrose:sucrose 1-fructosyltransferase</t>
+  </si>
+  <si>
+    <t>Transfers terminal (2→1)-linked-D-fructosyl group of an inulin chain onto O-6 position of the glucose residue of another inulin molecule</t>
+  </si>
+  <si>
+    <t>Randomly hydrolyzes (2→6)-β-D-fructofuranosidic linkages in (2→6)-β-D-fructans (levans) containing more than 3 fructose units</t>
+  </si>
+  <si>
+    <t>Acts on sucrose. Catalyzes fructotransferase reactions</t>
+  </si>
+  <si>
+    <t>Hydrolyzes inulin, levan, and sucrose</t>
+  </si>
+  <si>
+    <t>Degrades inulin-type fructans (EC 3.2.1.80) and some levans (EC 3.2.1.154). Sucrose inhibits enzyme.</t>
+  </si>
+  <si>
+    <t>Degrades β-D-galactosides and α-L-arabinosides</t>
+  </si>
+  <si>
+    <t>α-L-rhamnosidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.40</t>
+  </si>
+  <si>
+    <t>rhamnogalacturonan α-L-rhamnohydrolase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.174</t>
+  </si>
+  <si>
+    <t>L-Rhap-α-1,3-D-Apif -specific α-1,3-L-rhamnosidase</t>
+  </si>
+  <si>
+    <t>Mucin degradation. Acts on N-acetylglucosides and N-acetylgalactosides</t>
+  </si>
+  <si>
+    <t>Mucin degradation. Acts on hydraluronate, chondroitin, chondroitin 4- and 6-sulfates, and dermatan.</t>
+  </si>
+  <si>
+    <t>Mucin degradation</t>
+  </si>
+  <si>
+    <t>Winter &gt; Spring</t>
+  </si>
+  <si>
+    <t>Eukaryotic enzymes (includes mammals and fungi (bacterial is GT5)). Does this help fungi survive hib because glycogen is an NRG source for microbesm</t>
+  </si>
+  <si>
+    <t>Buschiazzo 2004, Ball 2011, Chikwana 2013</t>
+  </si>
+  <si>
+    <t>endoglucanase</t>
+  </si>
+  <si>
+    <t>endo-β-1,3(4)-glucanase / lichenase-laminarinase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.6</t>
+  </si>
+  <si>
+    <t>cellobiohydrolase</t>
+  </si>
+  <si>
+    <t>xyloglucan-specific endo-β-1,4-glucanase / endo-xyloglucanase</t>
+  </si>
+  <si>
+    <t>exo-β-glucosaminidase</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.165</t>
+  </si>
+  <si>
+    <t>endo-β-1,4-glucanase (xanthanase)</t>
+  </si>
+  <si>
+    <t>Degrades laminarin, lichenin and cereal D-glucans</t>
+  </si>
+  <si>
+    <t>Wide specificity for β-D-glucosides. Some examples also hydrolyse one or more of the following: β-D-galactosides, α-L-arabinosides, β-D-xylosides, and β-D-fucosides</t>
+  </si>
+  <si>
+    <t>Acts on lichenin and cereal β-D-glucans, but not on β-D-glucans containing only 1,3- or 1,4-bonds</t>
+  </si>
+  <si>
+    <t>Specific for xyloglucan; doesn't hydrolyse other cell-wall components.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrolyzes chitosan and chitosan oligosaccharides </t>
+  </si>
+  <si>
+    <t>Not in 2 spring</t>
+  </si>
+  <si>
+    <t>UDP-GlcNAc: peptide β-N-acetylglucosaminyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.255</t>
+  </si>
+  <si>
+    <t>UDP-Glc: peptide N-β-glucosyltransferase</t>
+  </si>
+  <si>
+    <t>Involved in eukaryotic post-translation modification of proteins (transfer O-GlcNAc onto proteins)</t>
+  </si>
+  <si>
+    <t>sucrose synthase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.13</t>
+  </si>
+  <si>
+    <t>sucrose-phosphate synthase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.14</t>
+  </si>
+  <si>
+    <t>α-glucosyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.52</t>
+  </si>
+  <si>
+    <t>lipopolysaccharide N-acetylglucosaminyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.56</t>
+  </si>
+  <si>
+    <t>GDP-Man: Man1GlcNAc2-PP-dolichol α-1,3-mannosyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.132</t>
+  </si>
+  <si>
+    <t>GDP-Man: Man3GlcNAc2-PP-dolichol/Man4GlcNAc2-PP-dolichol α-1,2-mannosyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.131</t>
+  </si>
+  <si>
+    <t>digalactosyldiacylglycerol synthase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.141</t>
+  </si>
+  <si>
+    <t>diglucosyl diacylglycerol synthase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.208</t>
+  </si>
+  <si>
+    <t>trehalose phosphorylase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.231</t>
+  </si>
+  <si>
+    <t>NDP-Glc: α-glucose α-glucosyltransferase / α,α-trehalose synthase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.245</t>
+  </si>
+  <si>
+    <t>GDP-Man: Man2GlcNAc2-PP-dolichol α-1,6-mannosyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.257</t>
+  </si>
+  <si>
+    <t>UDP-GlcNAc: 2-deoxystreptamine α-N-acetylglucosaminyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.283</t>
+  </si>
+  <si>
+    <t>UDP-GlcNAc: ribostamycin α-N-acetylglucosaminyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.285</t>
+  </si>
+  <si>
+    <t>UDP-Gal α-galactosyltransferase</t>
+  </si>
+  <si>
+    <t>UDP-Xyl α-xylosyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.2.-</t>
+  </si>
+  <si>
+    <t>UDP-GlcA α-glucuronyltransferase</t>
+  </si>
+  <si>
+    <t>UDP-Glc α-glucosyltransferase</t>
+  </si>
+  <si>
+    <t>UDP-GalNAc: GalNAc-PP-Und α-1,3-N-acetylgalactosaminyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.306</t>
+  </si>
+  <si>
+    <t>UDP-GalNAc: N,N'-diacetylbacillosaminyl-PP-Und α-1,3-N-acetylgalactosaminyltransferase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.290</t>
+  </si>
+  <si>
+    <t>ADP-dependent α-maltose-1-phosphate synthase</t>
+  </si>
+  <si>
+    <t>EC 2.4.1.342</t>
+  </si>
+  <si>
+    <t>Although UDP is generally considered to be the preferred nucleoside diphosphate for sucrose synthase, numerous studies have shown that ADP serves as an effective acceptor molecule to produce ADP-glucose</t>
+  </si>
+  <si>
+    <t>Has dual role in producing both UDP-glucose (necessary for cell wall and glycoprotein biosynthesis) and ADP-glucose (necessary for starch biosynthesis)</t>
+  </si>
+  <si>
+    <t>Not specific for UDP-glucose; can use ADP-glucose and GDP-glucose as substrates. While the reaction catalysed by this enzyme is reversible, the enzyme usually works in concert with EC 3.1.3.24, sucrose-phosphate phosphatase, to form sucrose, making the above reaction essentially irreversible</t>
+  </si>
+  <si>
+    <t>Involved in biosynthesis of polyglycerol phosphate teichoic acids in bacterial cell walls</t>
+  </si>
+  <si>
+    <t>Transfers N-acetylglucosaminyl residues to a D-galactose residue in the partially completed lipopolysaccharide core</t>
+  </si>
+  <si>
+    <t>Part of dolichol pathway</t>
+  </si>
+  <si>
+    <t>Biosynthesis of asparagine-linked glycoproteins utilizes a dolichyl diphosphate-linked glycosyl donor, which is assembled by the series of membrane-bound glycosyltransferases that comprise the dolichol pathway </t>
+  </si>
+  <si>
+    <t>Involved in biosynthesis of several aminocyclitol antibiotics (e.g. kanamycin, butirosin, neomycin and ribostamycin)</t>
+  </si>
+  <si>
+    <t>Involved in biosynthesis of the O-polysaccharide repeating unit of E. coli serotype O86.</t>
+  </si>
+  <si>
+    <t>Part of bacterial N-linked glycosylation pathway</t>
+  </si>
+  <si>
+    <t>Not in eCAMI</t>
+  </si>
+  <si>
+    <t>EC 3.2.1.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,16 +1029,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -418,15 +1093,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E237DDC-612D-435C-B42D-9015223A018E}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1458,4 +2210,2082 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDA5AC4-ED18-4B68-BB57-CB6D824ACEB3}">
+  <dimension ref="A1:J111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="8.21875" customWidth="1"/>
+    <col min="5" max="5" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="J4" s="38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" s="31"/>
+    </row>
+    <row r="9" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" s="44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J13" s="44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="39" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="31"/>
+    </row>
+    <row r="27" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="J27" s="31"/>
+    </row>
+    <row r="28" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="J28" s="31"/>
+    </row>
+    <row r="29" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="42" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="G35" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="G37" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="39" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="G38" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="G39" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="G40" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="39" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="G41" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G43" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I43" s="17"/>
+      <c r="J43" s="39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="G44" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="G45" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I45" s="17"/>
+      <c r="J45" s="39" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F48" s="17"/>
+      <c r="G48" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="39" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="G49" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="39" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="39" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="G54" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I54" s="17"/>
+      <c r="J54" s="39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="F55" s="25"/>
+      <c r="G55" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F56" s="17"/>
+      <c r="G56" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="25"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F57" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="G57" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="F58" s="12"/>
+      <c r="G58" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J59" s="31"/>
+    </row>
+    <row r="60" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J60" s="31"/>
+    </row>
+    <row r="61" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="J61" s="31"/>
+    </row>
+    <row r="62" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="J62" s="31"/>
+    </row>
+    <row r="63" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="J63" s="31"/>
+    </row>
+    <row r="64" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="J64" s="31"/>
+    </row>
+    <row r="65" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J65" s="31"/>
+    </row>
+    <row r="66" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="J66" s="29"/>
+    </row>
+    <row r="67" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="28"/>
+    </row>
+    <row r="68" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E68" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="H68" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="J68" s="32"/>
+    </row>
+    <row r="69" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F69" s="17"/>
+      <c r="G69" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I69" s="17"/>
+      <c r="J69" s="39" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="F70" s="17"/>
+      <c r="G70" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H70" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I70" s="17"/>
+      <c r="J70" s="39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="F71" s="12"/>
+      <c r="G71" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="J72" s="44" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E73" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="G73" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="J73" s="38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="J74" s="28"/>
+    </row>
+    <row r="75" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J75" s="31"/>
+    </row>
+    <row r="76" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="J76" s="29"/>
+    </row>
+    <row r="77" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="J77" s="33"/>
+    </row>
+    <row r="78" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="G78" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="J78" s="44" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="26"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="F79" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="G79" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H79" s="26"/>
+      <c r="I79" s="26"/>
+      <c r="J79" s="36" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E80" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="G80" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J80" s="44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E81" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="G81" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J81" s="44" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="26"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="F82" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="G82" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H82" s="26"/>
+      <c r="I82" s="26"/>
+      <c r="J82" s="36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E83" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G83" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J83" s="44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E84" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G84" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J84" s="44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E85" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="G85" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J85" s="44" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E86" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="G86" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J86" s="38" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="I87" s="6"/>
+      <c r="J87" s="28"/>
+    </row>
+    <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="G88" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="H88" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="J88" s="44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E89" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="G89" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H89" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="J89" s="44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E90" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G90" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H90" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="J90" s="44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="26"/>
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="F91" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="G91" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H91" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="I91" s="26"/>
+      <c r="J91" s="36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E92" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="G92" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H92" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="J92" s="44" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="26"/>
+      <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="F93" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="G93" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H93" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="I93" s="26"/>
+      <c r="J93" s="36" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="26"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="F94" s="26"/>
+      <c r="G94" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H94" s="26"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="36" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E95" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G95" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H95" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="J95" s="44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E96" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="G96" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J96" s="44" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="G97" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J97" s="44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E98" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="G98" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J98" s="44" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E99" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="F99" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G99" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J99" s="44" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E100" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="G100" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H100" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="J100" s="44" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E101" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="G101" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J101" s="44" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E102" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G102" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J102" s="44" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="26"/>
+      <c r="B103" s="26"/>
+      <c r="C103" s="26"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="F103" s="26"/>
+      <c r="G103" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H103" s="26"/>
+      <c r="I103" s="26"/>
+      <c r="J103" s="36" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E104" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="G104" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J104" s="44" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E105" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="F105" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="G105" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H105" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="J105" s="44" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E106" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="G106" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H106" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="J106" s="44" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="26"/>
+      <c r="B107" s="26"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="F107" s="26"/>
+      <c r="G107" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="36" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B108" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E108" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="F108" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="G108" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="J108" s="49" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E109" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="F109" s="50"/>
+      <c r="G109" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="J109" s="51" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F111" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>